<commit_message>
Revised for class labels and add schema.org prefix.
</commit_message>
<xml_diff>
--- a/data/co-est2019-annres-sdd.xlsx
+++ b/data/co-est2019-annres-sdd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamie/Data/Whyis_Demo_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamie/opt/whyis_census_demo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2506BFDE-89BF-B645-BB5D-BC7653138079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2F84B54-DE99-CD46-80AF-7FFAB1E479B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2020" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary Mapping" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
   <si>
     <t>Column</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>{{{{row.State.replace(' ','_')}}}}_population</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>http://schema.org/</t>
   </si>
 </sst>
 </file>
@@ -660,8 +666,8 @@
   </sheetPr>
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="241" zoomScaleNormal="241" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScale="241" zoomScaleNormal="241" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
@@ -1059,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2A108F-5264-9442-8FE9-E0785C39EE7A}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1134,6 +1140,14 @@
         <v>73</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{663BA74F-01DC-E141-8A60-AA744D1D2595}"/>
@@ -1143,6 +1157,7 @@
     <hyperlink ref="B6" r:id="rId5" xr:uid="{4DED9595-4C7E-1A4B-9454-CA4648BFDAEB}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{FEB6D3B8-DA9B-D844-BD86-61FB95B8DA70}"/>
     <hyperlink ref="B8" r:id="rId7" xr:uid="{72C22DAE-C071-C744-9F1D-C128FB9FF7F1}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{5FE95B84-EB65-5E47-86AA-5455C4CFAE0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed county population URIs and added the dbpedia prefetch agent (commented out)
</commit_message>
<xml_diff>
--- a/data/co-est2019-annres-sdd.xlsx
+++ b/data/co-est2019-annres-sdd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamie/opt/whyis_census_demo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2F84B54-DE99-CD46-80AF-7FFAB1E479B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F3CF88-9C02-1647-BA59-A71E493A7BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary Mapping" sheetId="2" r:id="rId1"/>
@@ -270,13 +270,13 @@
     <t>{{{{row.County.replace(' ','_')}}}}_fips</t>
   </si>
   <si>
-    <t>{{{{row.State.replace(' ','_')}}}}_population</t>
-  </si>
-  <si>
     <t>schema</t>
   </si>
   <si>
     <t>http://schema.org/</t>
+  </si>
+  <si>
+    <t>{{{{row.County.replace(' ','_')}}}}_population</t>
   </si>
 </sst>
 </file>
@@ -666,8 +666,8 @@
   </sheetPr>
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView zoomScale="241" zoomScaleNormal="241" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="241" zoomScaleNormal="241" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
@@ -858,7 +858,7 @@
         <v>55</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -1067,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2A108F-5264-9442-8FE9-E0785C39EE7A}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1142,10 +1142,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for direct triples.
</commit_message>
<xml_diff>
--- a/data/co-est2019-annres-sdd.xlsx
+++ b/data/co-est2019-annres-sdd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamie/opt/whyis_census_demo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F3CF88-9C02-1647-BA59-A71E493A7BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C8A265-4D59-0748-B513-530B4C7936BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary Mapping" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="82">
   <si>
     <t>Column</t>
   </si>
@@ -249,9 +249,6 @@
     <t>http://dbpedia.org/ontology/</t>
   </si>
   <si>
-    <t>sio:Identifier,dbo:fipsCode</t>
-  </si>
-  <si>
     <t>skos:notation</t>
   </si>
   <si>
@@ -261,15 +258,6 @@
     <t>http://www.w3.org/2004/02/skos/core#</t>
   </si>
   <si>
-    <t>{{{{row.State.replace(' ','_')}}}}_fips</t>
-  </si>
-  <si>
-    <t>{{{{row.State.replace(' ','_')}}}}_abbr</t>
-  </si>
-  <si>
-    <t>{{{{row.County.replace(' ','_')}}}}_fips</t>
-  </si>
-  <si>
     <t>schema</t>
   </si>
   <si>
@@ -277,6 +265,24 @@
   </si>
   <si>
     <t>{{{{row.County.replace(' ','_')}}}}_population</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Predicate</t>
+  </si>
+  <si>
+    <t>dbo:fipsCode</t>
+  </si>
+  <si>
+    <t>rdfs:label</t>
+  </si>
+  <si>
+    <t>??cty</t>
+  </si>
+  <si>
+    <t>??st</t>
   </si>
 </sst>
 </file>
@@ -664,11 +670,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="241" zoomScaleNormal="241" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P7" sqref="P7"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -676,22 +682,23 @@
     <col min="1" max="1" width="17.83203125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" customWidth="1"/>
-    <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" customWidth="1"/>
+    <col min="4" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.6640625" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.33203125" customWidth="1"/>
-    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.6640625" customWidth="1"/>
+    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.33203125" customWidth="1"/>
+    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -704,203 +711,266 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>55</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="E2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="5"/>
+      <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="5" t="s">
-        <v>63</v>
-      </c>
+      <c r="J2" s="5"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O2" s="5"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="12"/>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="5"/>
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="5" t="s">
-        <v>62</v>
-      </c>
+      <c r="J3" s="5"/>
       <c r="K3" s="1"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L3" s="5"/>
+      <c r="M3" s="1"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="12"/>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="1"/>
+      <c r="J4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="2"/>
+      <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="14"/>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O4" s="2"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="14"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="2"/>
+      <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="5"/>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O5" s="2"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="5"/>
+    </row>
+    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="J6" s="5" t="s">
+      <c r="H6" s="5"/>
+      <c r="L6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="N6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="M6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="P6" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="R7" s="12"/>
+    </row>
+    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>71</v>
+      <c r="E8" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>70</v>
+      </c>
+      <c r="R8" s="12"/>
+    </row>
+    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="P9" s="12" t="s">
-        <v>76</v>
+      <c r="E9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="R9" s="12"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="12" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -908,12 +978,9 @@
     <mergeCell ref="B5:C5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{E4526E39-6CD3-F045-8E4E-496447B5274A}"/>
-    <hyperlink ref="P3" r:id="rId2" xr:uid="{3F0399B2-E1FF-FB4D-A5B2-E619866B1D29}"/>
-    <hyperlink ref="P7" r:id="rId3" display="http://dbpedia.org/resource/{{{{row.State.replace(' ','_')}}}}" xr:uid="{1DAC540D-6813-ED40-A7BD-66CF59466D09}"/>
-    <hyperlink ref="P8" r:id="rId4" display="http://dbpedia.org/resource/{{{{row.State.replace(' ','_')}}}}" xr:uid="{155D9F14-D359-0A47-A536-1FF051C8AF3F}"/>
-    <hyperlink ref="P9" r:id="rId5" display="http://dbpedia.org/resource/%7b%7b%7b%7brow.State.replace(' ','_')%7d%7d%7d%7d" xr:uid="{B6BC31BC-7F17-6244-A21C-0ED174FC8BB7}"/>
-    <hyperlink ref="P6" r:id="rId6" display="http://dbpedia.org/resource/%7b%7b%7b%7brow.State.replace(' ','_')%7d%7d%7d%7d" xr:uid="{EB847493-9227-3A4F-BFC9-3539D434B612}"/>
+    <hyperlink ref="R6" r:id="rId1" display="http://dbpedia.org/resource/%7b%7b%7b%7brow.State.replace(' ','_')%7d%7d%7d%7d" xr:uid="{EB847493-9227-3A4F-BFC9-3539D434B612}"/>
+    <hyperlink ref="R10" r:id="rId2" xr:uid="{A23C4E85-02F1-2E44-84A4-23218F390332}"/>
+    <hyperlink ref="R11" r:id="rId3" xr:uid="{CFB80585-4C2C-C149-91FA-F576C9E7BB5A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1134,18 +1201,18 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>